<commit_message>
minor changes to protocole attribution
</commit_message>
<xml_diff>
--- a/PROTOCOLE_attrib/PROTOCOLE_ATTRIBUTION_AuRA.xlsx
+++ b/PROTOCOLE_attrib/PROTOCOLE_ATTRIBUTION_AuRA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\RESEARCH\Lutralutra_PhD\Chap1_connectivity\FrenchOtters\PROTOCOLE_attrib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lacombe\Lutralutra\Chap1_connectivity\FrenchOtters\PROTOCOLE_attrib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0101D431-ADC5-4CD2-ABAB-BB48E67880EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3C3512-AD41-4EA8-8B62-E5244F7B0CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7CA4A75F-F0CD-4FC7-89F2-0F28F629AD78}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7CA4A75F-F0CD-4FC7-89F2-0F28F629AD78}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>PROTOCOLE</t>
   </si>
@@ -54,9 +54,6 @@
     <t>COMMENTAIRE</t>
   </si>
   <si>
-    <t>PRIORITÉ</t>
-  </si>
-  <si>
     <t>Présence seule</t>
   </si>
   <si>
@@ -138,19 +135,79 @@
     <t>"GROUPE JEUNES NATURE"</t>
   </si>
   <si>
-    <t>AUTRES TRANSECTS</t>
-  </si>
-  <si>
-    <t>"X00 M"|"X00M"</t>
-  </si>
-  <si>
-    <t>De nombreuses cellules mentionnent une distance parcourue lors de la prospection. Nous avons décidé de garder ces cellules et de les noter comme une prospection</t>
-  </si>
-  <si>
     <t>SUIVI RDE</t>
   </si>
   <si>
     <t>"SUIVI RDE"</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>UICN</t>
+  </si>
+  <si>
+    <t>CPO</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>PCS</t>
+  </si>
+  <si>
+    <t>GJN</t>
+  </si>
+  <si>
+    <t>RDE</t>
+  </si>
+  <si>
+    <t>OPP</t>
+  </si>
+  <si>
+    <t>PÉRIODE</t>
+  </si>
+  <si>
+    <t>2011-2023</t>
+  </si>
+  <si>
+    <t>2009-2023</t>
+  </si>
+  <si>
+    <t>2011-2012</t>
+  </si>
+  <si>
+    <t>2009-2011</t>
+  </si>
+  <si>
+    <t>2013-2012, 2021</t>
+  </si>
+  <si>
+    <t>2009-2017, 2019-2020, 2022</t>
+  </si>
+  <si>
+    <t>2011-2016</t>
+  </si>
+  <si>
+    <t>2018-2022</t>
+  </si>
+  <si>
+    <t>2019, 2023</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -186,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -194,11 +251,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -243,26 +310,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{112CD3B8-C868-4B27-B160-DB7EAFEAA94E}" name="Tableau1" displayName="Tableau1" ref="A1:H14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:H14" xr:uid="{112CD3B8-C868-4B27-B160-DB7EAFEAA94E}"/>
-  <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{8344113E-FB9F-429C-8627-2BE342DF5669}" name="PRIORITÉ" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{3041AC12-B8BD-4635-94A4-1BD523A699B9}" name="PROTOCOLE" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{C1AE1BC0-2BE4-48FE-A858-B47DB948D461}" name="TYPE DE PROTOCOLE" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{D2E44F51-3CEE-411B-BBB6-033CAF5398A0}" name="N TOTAL" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{82E73AA4-9FA4-47BD-8705-5FBD5A7F653B}" name="N PRÉSENCE" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{0B89AAAF-70F6-4B63-98E4-7254906E0660}" name="MOTS CLÉS (| = &quot;OU&quot; ;  &amp; = &quot;ET&quot; ;  ! = &quot;NON&quot; ; X = chiffre)" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{2622441C-FCA9-4482-9114-71E20A4FCDDC}" name="COMMENTAIRE" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{63335B66-67DC-4EE5-B9C2-B6953B7F012C}" name="DESCRIPTION (OPTIONNEL)" dataDxfId="0" dataCellStyle="Normal"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{112CD3B8-C868-4B27-B160-DB7EAFEAA94E}" name="Tableau1" displayName="Tableau1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:I13" xr:uid="{112CD3B8-C868-4B27-B160-DB7EAFEAA94E}"/>
+  <tableColumns count="9">
+    <tableColumn id="8" xr3:uid="{8344113E-FB9F-429C-8627-2BE342DF5669}" name="CODE" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{3041AC12-B8BD-4635-94A4-1BD523A699B9}" name="PROTOCOLE" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{C1AE1BC0-2BE4-48FE-A858-B47DB948D461}" name="TYPE DE PROTOCOLE" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{56836112-7592-4E4C-BC07-F4396DC03811}" name="PÉRIODE" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{D2E44F51-3CEE-411B-BBB6-033CAF5398A0}" name="N TOTAL" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{82E73AA4-9FA4-47BD-8705-5FBD5A7F653B}" name="N PRÉSENCE" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{0B89AAAF-70F6-4B63-98E4-7254906E0660}" name="MOTS CLÉS (| = &quot;OU&quot; ;  &amp; = &quot;ET&quot; ;  ! = &quot;NON&quot; ; X = chiffre)" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{2622441C-FCA9-4482-9114-71E20A4FCDDC}" name="COMMENTAIRE" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{63335B66-67DC-4EE5-B9C2-B6953B7F012C}" name="DESCRIPTION (OPTIONNEL)" dataDxfId="1" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -300,7 +368,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -406,7 +474,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -548,7 +616,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,281 +624,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A4A123-8F97-45E7-96DA-3B273C224F16}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="70.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="50" style="1" customWidth="1"/>
-    <col min="8" max="8" width="39.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="7" max="7" width="70.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="50" style="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="2">
+        <v>261</v>
+      </c>
+      <c r="F2" s="2">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2">
-        <f>25 + 238</f>
-        <v>263</v>
-      </c>
-      <c r="E2" s="2">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="1">
+        <v>995</v>
+      </c>
+      <c r="F3" s="1">
+        <v>48</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
-        <v>999</v>
-      </c>
-      <c r="E3" s="1">
-        <v>48</v>
-      </c>
-      <c r="F3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="1">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="1">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1">
-        <v>110</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="1">
         <v>74</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1">
+        <v>98</v>
+      </c>
+      <c r="F7" s="1">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="1">
+        <v>133</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1">
+        <v>69</v>
+      </c>
+      <c r="F9" s="1">
+        <v>54</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2020</v>
+      </c>
+      <c r="E10" s="1">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="1">
+        <v>32</v>
+      </c>
+      <c r="F11" s="1">
+        <v>22</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1">
-        <v>235</v>
-      </c>
-      <c r="E7" s="1">
-        <v>24</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1">
-        <v>133</v>
-      </c>
-      <c r="E8" s="1">
-        <v>44</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="1">
-        <v>70</v>
-      </c>
-      <c r="E9" s="1">
-        <v>55</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="1">
-        <v>21</v>
-      </c>
-      <c r="E10" s="1">
-        <v>18</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="D12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1">
-        <v>32</v>
-      </c>
-      <c r="E11" s="1">
-        <v>22</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="1">
-        <v>238</v>
-      </c>
-      <c r="E12" s="1">
-        <v>99</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1">
-        <v>10760</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1">
-        <v>2438</v>
+      <c r="F13" s="1">
+        <v>2378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>